<commit_message>
Updated the TestWebsites (after destroying it) and finalising our ProjectPresentation
</commit_message>
<xml_diff>
--- a/TestWebsites.xlsx
+++ b/TestWebsites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kozminski.sharepoint.com/sites/MicrosoftProject438/Shared Documents/General/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{A1993D97-2B67-414D-B17B-13FE706D514D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C85583D0-D530-4C94-855D-38D477F7AABB}"/>
+  <xr:revisionPtr revIDLastSave="104" documentId="8_{A1993D97-2B67-414D-B17B-13FE706D514D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{731E0CC6-B9E2-428D-A7C0-BC65238E0329}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C2A4A56D-7472-4AB6-AF12-0E4382030C4B}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8880" xr2:uid="{C2A4A56D-7472-4AB6-AF12-0E4382030C4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Real" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>https://www.bbc.com/news/world-europe-61742736</t>
   </si>
@@ -99,6 +99,120 @@
   </si>
   <si>
     <t>https://www.reuters.com/markets/europe/chinas-producer-inflation-eases-14-month-low-may-2022-06-10/</t>
+  </si>
+  <si>
+    <t>https://100percentfedup.com/oops-traitor-and-former-trump-education-sec-betsy-devos-trashes-trump-while-simultaneously-funding-gop-governor-candidate-gunning-for-trump-endorsement/</t>
+  </si>
+  <si>
+    <t>https://100percentfedup.com/the-biden-regime-claimed-that-their-disinformation-board-was-just-for-advisory-purposes-newly-released-documents-paint-a-darker-picture/</t>
+  </si>
+  <si>
+    <t>https://100percentfedup.com/lol-democrat-darling-rep-liz-cheney-gets-roasted-on-social-media-during-jan-6-witch-hunt-show-trial-liz-is-lying/</t>
+  </si>
+  <si>
+    <t>https://100percentfedup.com/finally-fauci-hints-at-when-he-is-going-to-retire-from-government/</t>
+  </si>
+  <si>
+    <t>https://100percentfedup.com/transgender-former-amazon-employee-goes-to-trial-for-stealing-over-100-million-capitol-one-customers-information/</t>
+  </si>
+  <si>
+    <t>https://100percentfedup.com/new-documents-show-biden-regimes-plan-to-send-migrants-to-cities-deeper-inside-u-s/</t>
+  </si>
+  <si>
+    <t>https://100percentfedup.com/washington-post-column-admits-dems-will-lose-hard-in-midterms-but-heres-the-twist/</t>
+  </si>
+  <si>
+    <t>https://pieceofmindful.com/2020/04/06/bombshell-who-coronavirus-pcr-test-primer-sequence-is-found-in-all-human-dna/</t>
+  </si>
+  <si>
+    <t>https://21stcenturywire.com/2022/06/10/vernon-coleman-the-death-of-health-care-in-britain/</t>
+  </si>
+  <si>
+    <t>https://21stcenturywire.com/2022/06/09/disinformation-board-leaked-documents-expose-agenda-behind-dhs-ministry-of-truth/</t>
+  </si>
+  <si>
+    <t>https://21stcenturywire.com/2022/06/08/was-the-pandemic-the-perfect-cover-for-the-great-reset/</t>
+  </si>
+  <si>
+    <t>https://21stcenturywire.com/2022/05/20/biden-orders-millions-of-monkeypox-vaccines-after-one-man-allegedly-infected/</t>
+  </si>
+  <si>
+    <t>https://21stcenturywire.com/2022/05/21/vernon-coleman-the-clock-is-ticking-loudly/</t>
+  </si>
+  <si>
+    <t>https://www.activistpost.com/2022/06/pfizer-ceo-head-of-cia-facebook-vp-other-elites-secretly-meeting-in-dc-corporate-media-is-silent.html</t>
+  </si>
+  <si>
+    <t>https://americanlookout.com/report-new-management-at-cnn-preparing-to-fire-partisan-hosts/</t>
+  </si>
+  <si>
+    <t>https://americanlookout.com/propaganda-democrats-hire-professional-tv-producer-for-prime-time-january-6th-hearings/</t>
+  </si>
+  <si>
+    <t>https://americanlookout.com/poll-finds-most-americans-believe-trump-is-not-responsible-for-january-6th/</t>
+  </si>
+  <si>
+    <t>https://americanlookout.com/report-john-deere-moving-part-of-production-from-iowa-to-mexico/</t>
+  </si>
+  <si>
+    <t>https://edition.cnn.com/2022/05/26/business/russia-economy-ruble-interest-rates/index.html</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2022/06/09/stock-market-news-open-to-close.html</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2022/06/10/flu-hepatitis-monkeypox-diseases-suppressed-during-covid-are-back.html</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2022/06/10/investment-banks-say-its-time-to-get-back-into-china-with-goldman-naming-10-top-stocks.html</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2022/06/10/klarna-ceo-defends-business-despite-massive-losses-and-layoffs.html</t>
+  </si>
+  <si>
+    <t>https://edition.cnn.com/2022/06/09/americas/dom-phillips-bruno-pereira-missing-suspect-intl-latam/index.html</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2022/06/10/ai-gurus-are-leaving-big-tech-to-work-on-buzzy-new-start-ups.html</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2022/06/10/carrie-lam-says-hong-kong-hasnt-become-just-another-chinese-city.html</t>
+  </si>
+  <si>
+    <t>https://edition.cnn.com/2022/06/08/americas/maduro-ankara-analysis-latam/index.html</t>
+  </si>
+  <si>
+    <t>https://www.cnbc.com/2022/06/10/tesla-cancels-three-june-online-hiring-events-for-china.html</t>
+  </si>
+  <si>
+    <t>https://edition.cnn.com/2022/06/10/politics/alejandro-mayorkas-interview-cnntv/index.html</t>
+  </si>
+  <si>
+    <t>https://www.politico.com/news/2022/06/09/cheney-scott-perry-jan-6-hearing-00038724</t>
+  </si>
+  <si>
+    <t>https://www.washingtonpost.com/world/2022/06/10/russia-putin-peter-the-great-ukraine-war/?itid=mr_world_2</t>
+  </si>
+  <si>
+    <t>https://www.washingtonpost.com/world/2022/06/09/china-rumors-xi-covid-politics/?itid=mr_world_3</t>
+  </si>
+  <si>
+    <t>https://www.washingtonpost.com/world/2022/06/09/who-sago-covid-origins/?itid=mr_world_4</t>
+  </si>
+  <si>
+    <t>https://www.politico.com/news/magazine/2022/06/10/ruth-bader-ginsburg-retire-legacy-00038638</t>
+  </si>
+  <si>
+    <t>https://www.washingtonpost.com/world/2022/06/09/belgium-king-philippe-democratic-republic-congo-colonialism/?itid=mr_world_5</t>
+  </si>
+  <si>
+    <t>https://www.politico.com/news/2022/06/10/chesa-boudin-progressive-agenda-california-00038675</t>
+  </si>
+  <si>
+    <t>https://www.politico.com/news/2022/06/09/biden-abortion-00038565</t>
+  </si>
+  <si>
+    <t>https://www.politico.com/sponsored-content/2022/05/seizing-the-next-revolution?utm_source=native&amp;utm_medium=hp</t>
   </si>
 </sst>
 </file>
@@ -461,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB95F7AF-15E0-4798-95A2-B4DAD704A230}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,6 +631,106 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -530,6 +744,26 @@
     <hyperlink ref="A8" r:id="rId7" xr:uid="{50679D02-7A41-4F0F-8C45-1317FB0C17FA}"/>
     <hyperlink ref="A9" r:id="rId8" xr:uid="{7AF373D7-EA5C-421A-BD35-DA797BA5130D}"/>
     <hyperlink ref="A10" r:id="rId9" xr:uid="{9527FF78-EA48-4B95-8816-281A4387CBFF}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{7CA14ACE-1914-42C0-9AEB-98FA0E126AEE}"/>
+    <hyperlink ref="A13" r:id="rId11" xr:uid="{15270D5C-3AB0-480B-BF0B-CD35EC2A2B89}"/>
+    <hyperlink ref="A14" r:id="rId12" xr:uid="{52398363-551F-4617-8EAB-20BABD4BAB37}"/>
+    <hyperlink ref="A15" r:id="rId13" xr:uid="{2FCC42F2-EC80-40A5-BC6A-8423AB43E95B}"/>
+    <hyperlink ref="A16" r:id="rId14" xr:uid="{3970D1DE-1953-4FD3-93C7-24A994A61E53}"/>
+    <hyperlink ref="A17" r:id="rId15" xr:uid="{DCD94BE9-3598-4574-AEE9-70199EF377BF}"/>
+    <hyperlink ref="A18" r:id="rId16" xr:uid="{C858BAEB-B561-42A0-9FAF-AF8D541CFABC}"/>
+    <hyperlink ref="A19" r:id="rId17" xr:uid="{9F54AD83-859B-4388-AF20-A0D36DF25180}"/>
+    <hyperlink ref="A12" r:id="rId18" xr:uid="{DF444352-DDEF-4B03-A216-31A035316EDA}"/>
+    <hyperlink ref="A22" r:id="rId19" xr:uid="{6D626EC2-B653-45A2-BCEB-9862BB9F9FD7}"/>
+    <hyperlink ref="A21" r:id="rId20" xr:uid="{4E370B0D-854D-4E3C-821E-5DB955D9F9A7}"/>
+    <hyperlink ref="A20" r:id="rId21" xr:uid="{C19B436E-39AB-410E-95B1-3BD470B5BBE4}"/>
+    <hyperlink ref="A27" r:id="rId22" xr:uid="{D47BBBBF-C6D0-4831-865B-369B448CD406}"/>
+    <hyperlink ref="A28" r:id="rId23" xr:uid="{0697A62B-79EC-45D5-A455-648B2C2283CF}"/>
+    <hyperlink ref="A23" r:id="rId24" xr:uid="{E07EC0CE-829D-4352-B437-95DDB01AA983}"/>
+    <hyperlink ref="A29" r:id="rId25" xr:uid="{E64906E3-4465-4BB5-8845-E97C4B3C05EC}"/>
+    <hyperlink ref="A24" r:id="rId26" xr:uid="{C909657E-ABA2-4C1A-BB17-FAF3596FC710}"/>
+    <hyperlink ref="A25" r:id="rId27" xr:uid="{8601109C-BD83-434A-843D-31E9745BF7BB}"/>
+    <hyperlink ref="A26" r:id="rId28" xr:uid="{D08900F3-FB12-451A-B672-A41E479B3494}"/>
+    <hyperlink ref="A30" r:id="rId29" xr:uid="{6540EA88-557A-4CA6-A57F-4A8EFBAE9D0E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -537,10 +771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F789474-E9DC-4AAF-A1ED-29A67C196F64}">
-  <dimension ref="A1:A12"/>
+  <dimension ref="A1:A30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,6 +837,96 @@
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -618,6 +942,24 @@
     <hyperlink ref="A10" r:id="rId9" xr:uid="{D5C71284-67F6-4B9D-B265-DF530A4BB393}"/>
     <hyperlink ref="A11" r:id="rId10" xr:uid="{75555E56-CC84-4095-A7B1-2F3ED80E5E3B}"/>
     <hyperlink ref="A12" r:id="rId11" xr:uid="{44952D6D-7181-497F-817C-AAB957E9B9E8}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{F9450563-AD97-42E1-9F0A-90BF2BDD71D5}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{F5F7A828-D54C-49DC-B77A-8513956F0803}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{4A3B42EB-EE14-4A1B-A464-B877D29B80C5}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{50874004-7843-4EF4-9314-7C9EEBF87251}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{B3B3CF5A-94E7-4996-BC2A-AF7609697B52}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{93DBC6AD-1C2C-4AC9-B60F-38A887F27C06}"/>
+    <hyperlink ref="A19" r:id="rId18" xr:uid="{688172DF-1EF1-4911-B0FD-8608279C30F0}"/>
+    <hyperlink ref="A23" r:id="rId19" xr:uid="{5DCFB396-1B10-49D7-A297-2F65180BAB69}"/>
+    <hyperlink ref="A20" r:id="rId20" xr:uid="{7C56200F-2209-4D3D-AF5B-FC335C231C6E}"/>
+    <hyperlink ref="A21" r:id="rId21" xr:uid="{E4D19377-7E5C-4724-B459-4BFE56B5AA91}"/>
+    <hyperlink ref="A22" r:id="rId22" xr:uid="{AA9AAD0E-C6F0-4CCA-A8D9-71D8FD5F2CCD}"/>
+    <hyperlink ref="A24" r:id="rId23" xr:uid="{F701E238-8F89-42A9-95F6-B92D2F4F930D}"/>
+    <hyperlink ref="A25" r:id="rId24" xr:uid="{138386A6-ADE5-4109-9AF2-E7442D00D1B5}"/>
+    <hyperlink ref="A26" r:id="rId25" xr:uid="{5C839BA6-5B6D-43DF-851D-03CCA83A570E}"/>
+    <hyperlink ref="A27" r:id="rId26" xr:uid="{29019B58-95BC-458E-80A3-26F4EB596A7A}"/>
+    <hyperlink ref="A28" r:id="rId27" xr:uid="{E3360145-CC80-4B03-BD24-C21633A9A09E}"/>
+    <hyperlink ref="A29" r:id="rId28" xr:uid="{779A3829-C2C6-476C-8A56-0EE7FAEE38BB}"/>
+    <hyperlink ref="A30" r:id="rId29" xr:uid="{0578786E-3419-4590-906E-B3A07177A2C9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>